<commit_message>
Deployed 30023a5 with MkDocs version: 1.5.2
</commit_message>
<xml_diff>
--- a/excel/experiment_data.xlsx
+++ b/excel/experiment_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sjsu0-my.sharepoint.com/personal/alavi_khan_sjsu_edu/Documents/Thessis/web_doc/tactile_surface/docs/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\tactile_surface\docs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{B6CC36E1-9323-4D46-BB8A-C1AFA51453DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BA9FA4B-EC27-4756-A3F0-59F69AB3F847}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7879BE-C849-4C71-B565-A3C588D3B6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>Experiment Name</t>
   </si>
@@ -239,14 +236,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -263,10 +265,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -532,331 +530,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="4" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="3" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.21875" customWidth="1"/>
     <col min="9" max="9" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deployed 2ffb31d with MkDocs version: 1.5.2
</commit_message>
<xml_diff>
--- a/excel/experiment_data.xlsx
+++ b/excel/experiment_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\tactile_surface\docs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7879BE-C849-4C71-B565-A3C588D3B6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B891613-8C61-4512-A6A9-1B14F6A22413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>SAC</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>- Agent learns to stabalize it in the same position. Model - 0</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>Partial State + Touch Vector - Joint Pos[2], Target_Pos[3],Sensor Array[400]-&gt; Image(20,20)</t>
+  </si>
+  <si>
+    <t>Abou the Agent Learning</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,10 +553,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -579,22 +579,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -605,22 +605,22 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -631,22 +631,22 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -657,22 +657,22 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -683,22 +683,22 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -711,16 +711,16 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -731,22 +731,22 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -757,22 +757,22 @@
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -783,22 +783,22 @@
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -809,22 +809,22 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>